<commit_message>
21 problems 20 ..
</commit_message>
<xml_diff>
--- a/Copy of Curious Freaks Coding Sheet.xlsx
+++ b/Copy of Curious Freaks Coding Sheet.xlsx
@@ -3989,10 +3989,10 @@
   <dimension ref="A1:G1505"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="72.37"/>
@@ -4789,7 +4789,7 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="21"/>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="32" t="s">
         <v>93</v>
       </c>
       <c r="C54" s="22" t="s">

</xml_diff>